<commit_message>
Algunos eventos más creados
Falta:
- el último evento
- ver la parte de mostrar en la tabla
- Métricas

Es decir: una banda
</commit_message>
<xml_diff>
--- a/TP5/Boceto Columnas.xlsx
+++ b/TP5/Boceto Columnas.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Tato\2022\SIM\TP-SIM\TP5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64151E54-6954-4C3B-BB8B-655B908DAEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF54BCB5-7923-42C4-90F6-1163592EB615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28665" yWindow="-135" windowWidth="24270" windowHeight="13050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$B$3:$X$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$B$3:$X$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Reloj (min)</t>
   </si>
@@ -212,6 +212,18 @@
   </si>
   <si>
     <t>nave 2</t>
+  </si>
+  <si>
+    <t>Libre</t>
+  </si>
+  <si>
+    <t>Atendido en caseta</t>
+  </si>
+  <si>
+    <t>Atendido en la nave 1</t>
+  </si>
+  <si>
+    <t>Ocupada</t>
   </si>
 </sst>
 </file>
@@ -234,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -265,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -562,7 +580,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -585,94 +603,102 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="60% - Énfasis1" xfId="1" builtinId="32"/>
@@ -956,16 +982,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AG14"/>
+  <dimension ref="A2:AG22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="B12:C13"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="10" width="15.6640625" customWidth="1"/>
     <col min="11" max="11" width="15.6640625" style="9" customWidth="1"/>
     <col min="12" max="18" width="15.6640625" customWidth="1"/>
@@ -981,73 +1007,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="35"/>
+      <c r="U2" s="35"/>
+      <c r="V2" s="35"/>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="35"/>
+      <c r="Z2" s="35"/>
+      <c r="AA2" s="35"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
     </row>
     <row r="3" spans="2:33" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17" t="s">
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17" t="s">
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17" t="s">
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17" t="s">
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="W3" s="17"/>
-      <c r="X3" s="18"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="32"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -1059,69 +1085,69 @@
       <c r="AG3" s="1"/>
     </row>
     <row r="4" spans="2:33" ht="60.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="26"/>
-      <c r="M4" s="10" t="s">
+      <c r="L4" s="24"/>
+      <c r="M4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10" t="s">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="R4" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="31" t="s">
+      <c r="S4" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="U4" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="V4" s="10" t="s">
+      <c r="V4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="11" t="s">
+      <c r="X4" s="25" t="s">
         <v>16</v>
       </c>
       <c r="Y4" s="1"/>
@@ -1135,276 +1161,463 @@
       <c r="AG4" s="1"/>
     </row>
     <row r="5" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="39">
+      <c r="B5" s="30"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="13">
         <v>1</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="13">
         <v>2</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="39">
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="13">
         <v>1</v>
       </c>
-      <c r="P5" s="39">
+      <c r="P5" s="13">
         <v>2</v>
       </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="32"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="21"/>
-    </row>
-    <row r="6" spans="2:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="2:33" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
+      <c r="Q5" s="28"/>
+      <c r="R5" s="28"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="28"/>
+      <c r="W5" s="28"/>
+      <c r="X5" s="26"/>
+    </row>
+    <row r="6" spans="2:33" s="10" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="40">
+        <v>0</v>
+      </c>
+      <c r="C6" s="40">
+        <v>0.12</v>
+      </c>
+      <c r="D6" s="40">
+        <v>5</v>
+      </c>
+      <c r="E6" s="41">
+        <v>5</v>
+      </c>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40"/>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.25</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>0.54</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" s="43">
+        <v>7</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>61</v>
+      </c>
+      <c r="R7" s="40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10">
+        <v>9</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.63</v>
+      </c>
+      <c r="J8" s="10">
+        <v>6</v>
+      </c>
+      <c r="K8" s="10">
+        <v>130</v>
+      </c>
+      <c r="L8" s="10">
+        <v>13</v>
+      </c>
+      <c r="Q8" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
+        <v>9</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="D9" s="10">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10">
+        <v>11</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="10">
+        <v>5</v>
+      </c>
+      <c r="H9" s="10">
+        <v>14</v>
+      </c>
+      <c r="K9" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:33" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="10">
+        <v>13</v>
+      </c>
+      <c r="L10" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:33" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="28" t="s">
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="28" t="s">
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="30"/>
-      <c r="O7" s="28" t="s">
+      <c r="N11" s="22"/>
+      <c r="O11" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="28" t="s">
+      <c r="P11" s="22"/>
+      <c r="Q11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="R7" s="29"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="7" t="s">
+      <c r="R11" s="21"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="U11" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="2:33" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="15" t="s">
+    <row r="12" spans="2:33" ht="68.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C12" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E12" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F12" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G12" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I12" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="33" t="s">
+      <c r="J12" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="31" t="s">
+      <c r="K12" s="17"/>
+      <c r="L12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="31" t="s">
+      <c r="M12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="N8" s="31" t="s">
+      <c r="N12" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="O8" s="31" t="s">
+      <c r="O12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="P8" s="31" t="s">
+      <c r="P12" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="Q8" s="31" t="s">
+      <c r="Q12" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="R8" s="33" t="s">
+      <c r="R12" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="S8" s="34"/>
-      <c r="T8" s="31" t="s">
+      <c r="S12" s="17"/>
+      <c r="T12" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="U8" s="11" t="s">
+      <c r="U12" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
-      <c r="R9" s="35"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="32"/>
-      <c r="U9" s="21"/>
-    </row>
-    <row r="10" spans="2:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="2:33" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12" t="s">
+    <row r="13" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="30"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="26"/>
+    </row>
+    <row r="14" spans="2:33" s="10" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="40">
+        <v>0</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+    </row>
+    <row r="15" spans="2:33" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="40">
+        <v>5</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+    </row>
+    <row r="16" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="14"/>
-    </row>
-    <row r="12" spans="2:33" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="15" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+    </row>
+    <row r="18" spans="1:12" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10" t="s">
+      <c r="C18" s="27"/>
+      <c r="D18" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10" t="s">
+      <c r="E18" s="27"/>
+      <c r="F18" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10" t="s">
+      <c r="I18" s="27"/>
+      <c r="J18" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="24"/>
-      <c r="L12" s="11"/>
-    </row>
-    <row r="13" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="2" t="s">
+      <c r="K18" s="23"/>
+      <c r="L18" s="25"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="4" t="s">
+      <c r="K19" s="11"/>
+      <c r="L19" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="2:33" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="R8:S9"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="J8:K9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="V4:V5"/>
-    <mergeCell ref="W4:W5"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="B17:L17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="Y2:AC2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="M2:P2"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:P4"/>
     <mergeCell ref="Q4:Q5"/>
@@ -1414,20 +1627,47 @@
     <mergeCell ref="I3:L3"/>
     <mergeCell ref="M3:P3"/>
     <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="Y2:AC2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="V4:V5"/>
+    <mergeCell ref="W4:W5"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="J12:K13"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="T12:T13"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="S4:S5"/>
+    <mergeCell ref="R12:S13"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="Q12:Q13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="22" orientation="portrait" r:id="rId1"/>

</xml_diff>